<commit_message>
Removed couchdb dependancy and made it work
</commit_message>
<xml_diff>
--- a/storage/EXAMENS.xlsx
+++ b/storage/EXAMENS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\var\www\nlims_controller_global\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D238F3F-6AAD-4768-9DAB-619696F8F109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895EA2EF-88B9-4223-AE2C-DDB339922FB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" activeTab="3" xr2:uid="{E4507F59-408D-4FB0-8A67-644CB3019B49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" xr2:uid="{E4507F59-408D-4FB0-8A67-644CB3019B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hématologie" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="221">
   <si>
     <t>Examens</t>
   </si>
@@ -388,12 +388,6 @@
     <t>pg/ml</t>
   </si>
   <si>
-    <t>&lt; 75 ans</t>
-  </si>
-  <si>
-    <t>&gt;= 75 ans</t>
-  </si>
-  <si>
     <t>PCT (Procalcitonine)</t>
   </si>
   <si>
@@ -683,6 +677,21 @@
   </si>
   <si>
     <t>Stool</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>expected turn around time</t>
+  </si>
+  <si>
+    <t>turn around time unit</t>
+  </si>
+  <si>
+    <t>measure type</t>
+  </si>
+  <si>
+    <t>interpretation</t>
   </si>
 </sst>
 </file>
@@ -1035,21 +1044,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1540243A-9CAA-4A08-A50C-1E94B4501B7C}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="35.578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.83984375" customWidth="1"/>
+    <col min="9" max="9" width="18.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1057,563 +1068,583 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="K1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="I2">
         <v>4000</v>
       </c>
-      <c r="F2">
+      <c r="J2">
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="I3">
         <v>4500000</v>
       </c>
-      <c r="F3">
+      <c r="J3">
         <v>5500000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1">
+      <c r="I4" s="1">
         <v>11</v>
       </c>
-      <c r="F4">
+      <c r="J4">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
-      </c>
-      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="I5">
         <v>35</v>
       </c>
-      <c r="F5">
+      <c r="J5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H6" t="s">
         <v>14</v>
       </c>
-      <c r="E6">
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="J6">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="K6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D7" t="s">
+        <v>208</v>
+      </c>
+      <c r="H7" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
+      <c r="I7">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="J7">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
+      <c r="K7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D8" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8" t="s">
         <v>18</v>
       </c>
-      <c r="E8">
+      <c r="I8">
         <v>80</v>
       </c>
-      <c r="F8">
+      <c r="J8">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>210</v>
-      </c>
-      <c r="D9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
-      </c>
-      <c r="D10" t="s">
+        <v>208</v>
+      </c>
+      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="E10">
+      <c r="I10">
         <v>32</v>
       </c>
-      <c r="F10">
+      <c r="J10">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D11" t="s">
+        <v>208</v>
+      </c>
+      <c r="H11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="I11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" t="s">
+      <c r="J11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D12" t="s">
+        <v>208</v>
+      </c>
+      <c r="H12" t="s">
         <v>12</v>
       </c>
-      <c r="E12">
+      <c r="I12">
         <v>50</v>
       </c>
-      <c r="F12">
+      <c r="J12">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D13" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" t="s">
         <v>12</v>
       </c>
-      <c r="E13">
+      <c r="I13">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="J13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
-      </c>
-      <c r="D14" t="s">
+        <v>208</v>
+      </c>
+      <c r="H14" t="s">
         <v>12</v>
       </c>
-      <c r="E14">
+      <c r="I14">
         <v>0</v>
       </c>
-      <c r="F14">
+      <c r="J14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>210</v>
-      </c>
-      <c r="D15" t="s">
+        <v>208</v>
+      </c>
+      <c r="H15" t="s">
         <v>12</v>
       </c>
-      <c r="E15">
+      <c r="I15">
         <v>4</v>
       </c>
-      <c r="F15">
+      <c r="J15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
-      </c>
-      <c r="D16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16" t="s">
         <v>12</v>
       </c>
-      <c r="E16">
+      <c r="I16">
         <v>17</v>
       </c>
-      <c r="F16">
+      <c r="J16">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
-      </c>
-      <c r="D17" t="s">
+        <v>208</v>
+      </c>
+      <c r="H17" t="s">
         <v>7</v>
       </c>
-      <c r="E17">
+      <c r="I17">
         <v>150000</v>
       </c>
-      <c r="F17">
+      <c r="J17">
         <v>450000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>210</v>
-      </c>
-      <c r="D18" t="s">
+        <v>208</v>
+      </c>
+      <c r="H18" t="s">
         <v>34</v>
       </c>
-      <c r="E18">
+      <c r="I18">
         <v>1</v>
       </c>
-      <c r="F18">
+      <c r="J18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>210</v>
-      </c>
-      <c r="D19" t="s">
+        <v>208</v>
+      </c>
+      <c r="H19" t="s">
         <v>34</v>
       </c>
-      <c r="E19">
+      <c r="I19">
         <v>5</v>
       </c>
-      <c r="F19">
+      <c r="J19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
-      </c>
-      <c r="C23" t="s">
+        <v>208</v>
+      </c>
+      <c r="G23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>210</v>
-      </c>
-      <c r="C24" t="s">
+        <v>208</v>
+      </c>
+      <c r="G24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>210</v>
-      </c>
-      <c r="C25" t="s">
+        <v>208</v>
+      </c>
+      <c r="G25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>210</v>
-      </c>
-      <c r="C26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>210</v>
-      </c>
-      <c r="C27" t="s">
+        <v>208</v>
+      </c>
+      <c r="G27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>210</v>
-      </c>
-      <c r="C28" t="s">
+        <v>208</v>
+      </c>
+      <c r="G28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>47</v>
       </c>
       <c r="B30" t="s">
-        <v>210</v>
-      </c>
-      <c r="D30" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30" t="s">
         <v>48</v>
       </c>
-      <c r="E30" t="s">
+      <c r="I30" t="s">
         <v>49</v>
       </c>
-      <c r="F30" t="s">
+      <c r="J30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
-      </c>
-      <c r="D31" t="s">
+        <v>209</v>
+      </c>
+      <c r="H31" t="s">
         <v>48</v>
       </c>
-      <c r="E31" t="s">
+      <c r="I31" t="s">
         <v>52</v>
       </c>
-      <c r="F31" t="s">
+      <c r="J31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
-      </c>
-      <c r="D32" t="s">
+        <v>209</v>
+      </c>
+      <c r="H32" t="s">
         <v>48</v>
       </c>
-      <c r="E32" t="s">
+      <c r="I32" t="s">
         <v>55</v>
       </c>
-      <c r="F32" t="s">
+      <c r="J32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
-      </c>
-      <c r="D33" t="s">
+        <v>209</v>
+      </c>
+      <c r="H33" t="s">
         <v>48</v>
       </c>
-      <c r="E33" t="s">
+      <c r="I33" t="s">
         <v>58</v>
       </c>
-      <c r="F33" t="s">
+      <c r="J33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
-      </c>
-      <c r="D34" t="s">
+        <v>209</v>
+      </c>
+      <c r="H34" t="s">
         <v>48</v>
       </c>
-      <c r="E34" t="s">
+      <c r="I34" t="s">
         <v>61</v>
       </c>
-      <c r="F34" t="s">
+      <c r="J34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
-      </c>
-      <c r="D35" t="s">
+        <v>209</v>
+      </c>
+      <c r="H35" t="s">
         <v>48</v>
       </c>
-      <c r="E35" t="s">
+      <c r="I35" t="s">
         <v>64</v>
       </c>
-      <c r="F35" t="s">
+      <c r="J35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{0033C87A-3718-419C-A4BE-90E537C70DEF}">
+      <formula1>"Auto Complete, Free Text, Numeric, Alpha Numeric"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1621,23 +1652,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378085E8-49BE-44FC-85B7-BE860EEC5B32}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="23.41796875" customWidth="1"/>
-    <col min="3" max="3" width="16.68359375" customWidth="1"/>
-    <col min="4" max="4" width="16.26171875" customWidth="1"/>
-    <col min="5" max="6" width="16.41796875" customWidth="1"/>
+    <col min="3" max="3" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.83984375" customWidth="1"/>
+    <col min="7" max="7" width="16.68359375" customWidth="1"/>
+    <col min="8" max="8" width="16.26171875" customWidth="1"/>
+    <col min="9" max="10" width="16.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1645,541 +1678,558 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="K1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
+      <c r="I2">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D3" t="s">
+        <v>209</v>
+      </c>
+      <c r="H3" t="s">
         <v>73</v>
       </c>
-      <c r="E3">
+      <c r="I3">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H4" t="s">
         <v>73</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" t="s">
         <v>77</v>
       </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="I5">
+        <v>1.5</v>
+      </c>
+      <c r="J5" t="s">
         <v>78</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H6" t="s">
         <v>77</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>79</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>80</v>
       </c>
-      <c r="G6" t="s">
+      <c r="K6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7" t="s">
         <v>77</v>
       </c>
-      <c r="E7" t="s">
+      <c r="I7" t="s">
         <v>81</v>
       </c>
-      <c r="F7" t="s">
+      <c r="J7" t="s">
         <v>82</v>
       </c>
-      <c r="G7" t="s">
+      <c r="K7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D8" t="s">
+        <v>209</v>
+      </c>
+      <c r="H8" t="s">
         <v>77</v>
       </c>
-      <c r="E8" t="s">
+      <c r="I8" t="s">
         <v>83</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
         <v>84</v>
       </c>
-      <c r="G8" t="s">
+      <c r="K8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H9" t="s">
         <v>77</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>85</v>
       </c>
-      <c r="F9">
+      <c r="J9">
         <v>130</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" t="s">
+        <v>209</v>
+      </c>
+      <c r="H10" t="s">
         <v>77</v>
       </c>
-      <c r="E10" t="s">
+      <c r="I10" t="s">
         <v>87</v>
       </c>
-      <c r="F10" t="s">
+      <c r="J10" t="s">
         <v>88</v>
       </c>
-      <c r="G10" t="s">
+      <c r="K10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>211</v>
-      </c>
-      <c r="D11" t="s">
+        <v>209</v>
+      </c>
+      <c r="H11" t="s">
         <v>77</v>
       </c>
-      <c r="E11" t="s">
+      <c r="I11" t="s">
         <v>89</v>
       </c>
-      <c r="F11" t="s">
+      <c r="J11" t="s">
         <v>90</v>
       </c>
-      <c r="G11" t="s">
+      <c r="K11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D12" t="s">
+        <v>209</v>
+      </c>
+      <c r="H12" t="s">
         <v>77</v>
       </c>
-      <c r="E12" t="s">
+      <c r="I12" t="s">
         <v>90</v>
       </c>
-      <c r="F12" t="s">
+      <c r="J12" t="s">
         <v>91</v>
       </c>
-      <c r="G12" t="s">
+      <c r="K12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D13" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" t="s">
         <v>77</v>
       </c>
-      <c r="E13" t="s">
+      <c r="I13" t="s">
         <v>92</v>
       </c>
-      <c r="F13">
+      <c r="J13">
         <v>11</v>
       </c>
-      <c r="G13" t="s">
+      <c r="K13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" t="s">
         <v>77</v>
       </c>
-      <c r="E14" t="s">
+      <c r="I14" t="s">
         <v>93</v>
       </c>
-      <c r="F14" t="s">
+      <c r="J14" t="s">
         <v>94</v>
       </c>
-      <c r="G14" t="s">
+      <c r="K14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" t="s">
+        <v>209</v>
+      </c>
+      <c r="H15" t="s">
         <v>96</v>
       </c>
-      <c r="E15" t="s">
+      <c r="I15" t="s">
         <v>97</v>
       </c>
-      <c r="F15" t="s">
+      <c r="J15" t="s">
         <v>98</v>
       </c>
-      <c r="G15" t="s">
+      <c r="K15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
-      </c>
-      <c r="D16" t="s">
+        <v>209</v>
+      </c>
+      <c r="H16" t="s">
         <v>96</v>
       </c>
-      <c r="E16" t="s">
+      <c r="I16" t="s">
         <v>99</v>
       </c>
-      <c r="F16" t="s">
+      <c r="J16" t="s">
         <v>100</v>
       </c>
-      <c r="G16" t="s">
+      <c r="K16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
-      </c>
-      <c r="D17" t="s">
+        <v>209</v>
+      </c>
+      <c r="H17" t="s">
         <v>102</v>
       </c>
-      <c r="E17">
+      <c r="I17">
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="J17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>211</v>
-      </c>
-      <c r="D18" t="s">
+        <v>209</v>
+      </c>
+      <c r="H18" t="s">
         <v>102</v>
       </c>
-      <c r="F18" t="s">
+      <c r="J18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>211</v>
-      </c>
-      <c r="D19" t="s">
+        <v>209</v>
+      </c>
+      <c r="H19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>211</v>
-      </c>
-      <c r="D20" t="s">
+        <v>209</v>
+      </c>
+      <c r="H20" t="s">
         <v>107</v>
       </c>
-      <c r="E20" t="s">
+      <c r="I20" t="s">
         <v>108</v>
       </c>
-      <c r="F20" t="s">
+      <c r="J20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
-      </c>
-      <c r="D21" t="s">
+        <v>209</v>
+      </c>
+      <c r="H21" t="s">
         <v>107</v>
       </c>
-      <c r="E21">
+      <c r="I21">
         <v>66</v>
       </c>
-      <c r="F21">
+      <c r="J21">
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>211</v>
-      </c>
-      <c r="D22" t="s">
+        <v>209</v>
+      </c>
+      <c r="H22" t="s">
         <v>77</v>
       </c>
-      <c r="E22" t="s">
+      <c r="I22" t="s">
         <v>112</v>
       </c>
-      <c r="F22" t="s">
+      <c r="J22" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>211</v>
-      </c>
-      <c r="D23" t="s">
+        <v>209</v>
+      </c>
+      <c r="H23" t="s">
         <v>102</v>
       </c>
-      <c r="F23" t="s">
+      <c r="J23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>211</v>
-      </c>
-      <c r="D24" t="s">
+        <v>209</v>
+      </c>
+      <c r="H24" t="s">
         <v>102</v>
       </c>
-      <c r="E24" t="s">
+      <c r="I24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>117</v>
       </c>
       <c r="B25" t="s">
-        <v>211</v>
-      </c>
-      <c r="D25" t="s">
+        <v>209</v>
+      </c>
+      <c r="H25" t="s">
         <v>118</v>
       </c>
-      <c r="E25">
+      <c r="I25">
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="J25">
         <v>300</v>
       </c>
-      <c r="G25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
-      </c>
-      <c r="D26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" t="s">
         <v>118</v>
       </c>
-      <c r="E26">
+      <c r="I26">
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="J26">
         <v>450</v>
       </c>
-      <c r="G26" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" t="s">
+        <v>209</v>
+      </c>
+      <c r="H27" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
+        <v>209</v>
+      </c>
+      <c r="H28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J28" t="s">
         <v>121</v>
       </c>
-      <c r="B27" t="s">
-        <v>211</v>
-      </c>
-      <c r="D27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
         <v>122</v>
       </c>
-      <c r="B28" t="s">
-        <v>211</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B29" t="s">
+        <v>209</v>
+      </c>
+      <c r="H29" t="s">
         <v>96</v>
       </c>
-      <c r="F28" t="s">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B29" t="s">
-        <v>211</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B30" t="s">
+        <v>209</v>
+      </c>
+      <c r="H30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" t="s">
-        <v>211</v>
-      </c>
-      <c r="D30" t="s">
-        <v>96</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{B6CC5FBC-8385-44EE-812B-2B39A1F2809E}">
+      <formula1>"Auto Complete, Free Text, Numeric, Alpha Numeric"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22ADCC3-18B4-430C-9ED3-8A2AA72287E2}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="21.26171875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2187,555 +2237,575 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="K1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2">
+        <v>70</v>
+      </c>
+      <c r="J2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
         <v>126</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3">
+        <v>70</v>
+      </c>
+      <c r="J3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>209</v>
+      </c>
+      <c r="H4" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" t="s">
+        <v>130</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" t="s">
+        <v>209</v>
+      </c>
+      <c r="H8" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" t="s">
+        <v>209</v>
+      </c>
+      <c r="H10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10">
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
+      <c r="H11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11">
+        <v>500</v>
+      </c>
+      <c r="J11">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" t="s">
+        <v>209</v>
+      </c>
+      <c r="H12" t="s">
+        <v>125</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" t="s">
+        <v>139</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" t="s">
         <v>210</v>
       </c>
-      <c r="D2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2">
-        <v>70</v>
-      </c>
-      <c r="F2">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="H15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15">
+        <v>135</v>
+      </c>
+      <c r="J15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" t="s">
         <v>210</v>
       </c>
-      <c r="D3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3">
-        <v>70</v>
-      </c>
-      <c r="F3">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
-      <c r="F4">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="H16" t="s">
+        <v>144</v>
+      </c>
+      <c r="I16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" t="s">
+        <v>210</v>
+      </c>
+      <c r="H17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17">
+        <v>97</v>
+      </c>
+      <c r="J17">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" t="s">
+        <v>210</v>
+      </c>
+      <c r="H18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I18" t="s">
+        <v>148</v>
+      </c>
+      <c r="J18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" t="s">
+        <v>210</v>
+      </c>
+      <c r="H19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" t="s">
+        <v>210</v>
+      </c>
+      <c r="H20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I20" t="s">
+        <v>152</v>
+      </c>
+      <c r="J20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B21" t="s">
+        <v>210</v>
+      </c>
+      <c r="H21" t="s">
+        <v>125</v>
+      </c>
+      <c r="I21" t="s">
+        <v>155</v>
+      </c>
+      <c r="J21" t="s">
         <v>130</v>
       </c>
-      <c r="B5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10">
-        <v>40</v>
-      </c>
-      <c r="F10">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" t="s">
-        <v>211</v>
-      </c>
-      <c r="D11" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11">
-        <v>500</v>
-      </c>
-      <c r="F11">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" t="s">
-        <v>211</v>
-      </c>
-      <c r="D13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" t="s">
-        <v>141</v>
-      </c>
-      <c r="F14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" t="s">
-        <v>212</v>
-      </c>
-      <c r="D15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E15">
-        <v>135</v>
-      </c>
-      <c r="F15">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B16" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D17" t="s">
-        <v>146</v>
-      </c>
-      <c r="E17">
-        <v>97</v>
-      </c>
-      <c r="F17">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" t="s">
-        <v>150</v>
-      </c>
-      <c r="F18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" t="s">
-        <v>212</v>
-      </c>
-      <c r="D19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" t="s">
-        <v>212</v>
-      </c>
-      <c r="D20" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" t="s">
-        <v>154</v>
-      </c>
-      <c r="F20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
         <v>156</v>
       </c>
-      <c r="B21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D21" t="s">
-        <v>127</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="B22" t="s">
+        <v>209</v>
+      </c>
+      <c r="H22" t="s">
         <v>157</v>
       </c>
-      <c r="F21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+      <c r="J22" t="s">
         <v>158</v>
       </c>
-      <c r="B22" t="s">
-        <v>211</v>
-      </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
         <v>159</v>
       </c>
-      <c r="F22" t="s">
+      <c r="B23" t="s">
+        <v>209</v>
+      </c>
+      <c r="H23" t="s">
+        <v>157</v>
+      </c>
+      <c r="J23" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
         <v>161</v>
       </c>
-      <c r="B23" t="s">
-        <v>211</v>
-      </c>
-      <c r="D23" t="s">
-        <v>159</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="B24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>164</v>
-      </c>
       <c r="B25" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>47</v>
       </c>
       <c r="B26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26">
+        <v>38</v>
+      </c>
+      <c r="J26">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" t="s">
+        <v>209</v>
+      </c>
+      <c r="H27" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27">
+        <v>60</v>
+      </c>
+      <c r="J27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" t="s">
+        <v>209</v>
+      </c>
+      <c r="H29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" t="s">
+        <v>209</v>
+      </c>
+      <c r="H30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+      <c r="G31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" t="s">
         <v>211</v>
       </c>
-      <c r="D26" t="s">
+      <c r="G32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" t="s">
+        <v>211</v>
+      </c>
+      <c r="H33" t="s">
+        <v>171</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B34" t="s">
+        <v>211</v>
+      </c>
+      <c r="H34" t="s">
+        <v>125</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B35" t="s">
+        <v>211</v>
+      </c>
+      <c r="H35" t="s">
         <v>48</v>
       </c>
-      <c r="E26">
-        <v>38</v>
-      </c>
-      <c r="F26">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>165</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" t="s">
         <v>211</v>
       </c>
-      <c r="D27" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27">
-        <v>60</v>
-      </c>
-      <c r="F27">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>166</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="G36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>167</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="G37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38" t="s">
         <v>211</v>
       </c>
-      <c r="D29" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>169</v>
-      </c>
-      <c r="B30" t="s">
-        <v>211</v>
-      </c>
-      <c r="D30" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" t="s">
-        <v>210</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="G38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" t="s">
-        <v>213</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B33" t="s">
-        <v>213</v>
-      </c>
-      <c r="D33" t="s">
-        <v>173</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>175</v>
-      </c>
-      <c r="B34" t="s">
-        <v>213</v>
-      </c>
-      <c r="D34" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>176</v>
-      </c>
-      <c r="B35" t="s">
-        <v>213</v>
-      </c>
-      <c r="D35" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>177</v>
-      </c>
-      <c r="B36" t="s">
-        <v>213</v>
-      </c>
-      <c r="C36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>178</v>
-      </c>
-      <c r="B37" t="s">
-        <v>213</v>
-      </c>
-      <c r="C37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>179</v>
-      </c>
-      <c r="B38" t="s">
-        <v>213</v>
-      </c>
-      <c r="C38" t="s">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{1AABA173-1840-4CD3-B40C-7980058AC08A}">
+      <formula1>"Auto Complete, Free Text, Numeric, Alpha Numeric"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2743,20 +2813,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5883E73-6570-469C-B00B-2AE9C0B4CDEF}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="37.83984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.83984375" customWidth="1"/>
+    <col min="8" max="8" width="21.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2764,222 +2836,244 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="K1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
         <v>180</v>
       </c>
-      <c r="B2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" t="s">
+        <v>184</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" t="s">
+        <v>213</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>189</v>
+      </c>
+      <c r="J10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>189</v>
+      </c>
+      <c r="I11">
+        <v>2001</v>
+      </c>
+      <c r="J11">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I12">
+        <v>4001</v>
+      </c>
+      <c r="J12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" t="s">
+        <v>189</v>
+      </c>
+      <c r="J13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" t="s">
         <v>181</v>
       </c>
-      <c r="B3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>188</v>
-      </c>
-      <c r="B8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>189</v>
-      </c>
-      <c r="B9" t="s">
-        <v>210</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>190</v>
-      </c>
-      <c r="B10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>191</v>
-      </c>
-      <c r="F10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" t="s">
-        <v>210</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>191</v>
-      </c>
-      <c r="E11">
-        <v>2001</v>
-      </c>
-      <c r="F11">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>190</v>
-      </c>
-      <c r="B12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
-        <v>191</v>
-      </c>
-      <c r="E12">
-        <v>4001</v>
-      </c>
-      <c r="F12">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>191</v>
-      </c>
-      <c r="F13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>194</v>
-      </c>
-      <c r="B14" t="s">
-        <v>183</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>195</v>
-      </c>
-      <c r="B15" t="s">
-        <v>183</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{90AEF74A-09D7-4B48-8FD8-3F15E7780BC3}">
+      <formula1>"Auto Complete, Free Text, Numeric, Alpha Numeric"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058C4361-8A64-4A1B-8C01-6330C5F7CB23}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="44.578125" customWidth="1"/>
     <col min="2" max="2" width="26.68359375" customWidth="1"/>
+    <col min="3" max="3" width="21.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2987,153 +3081,173 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="K1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="I2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I3" t="s">
         <v>196</v>
       </c>
-      <c r="B2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>209</v>
+      </c>
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="J4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
         <v>199</v>
       </c>
-      <c r="F4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
         <v>200</v>
       </c>
-      <c r="B5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5">
+      <c r="B6" t="s">
+        <v>209</v>
+      </c>
+      <c r="H6" t="s">
+        <v>201</v>
+      </c>
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="J6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
         <v>202</v>
       </c>
-      <c r="B6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B7" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7" t="s">
         <v>203</v>
       </c>
-      <c r="E6">
+      <c r="I7">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="J7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
         <v>204</v>
       </c>
-      <c r="B7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
         <v>205</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
         <v>206</v>
       </c>
-      <c r="B8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B10" t="s">
+        <v>209</v>
+      </c>
+      <c r="G10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
         <v>207</v>
       </c>
-      <c r="B9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
+      <c r="G11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B11" t="s">
-        <v>211</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{4135F017-CEC7-4C3E-806D-4174A0F0139B}">
+      <formula1>"Auto Complete, Free Text, Numeric, Alpha Numeric"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed updating of tests
</commit_message>
<xml_diff>
--- a/storage/EXAMENS.xlsx
+++ b/storage/EXAMENS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\var\www\nlims_controller_global\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F99CC5-D92E-4326-BEC5-FFEB62047D5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC4318C-B944-4B13-948A-2362675314EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" activeTab="4" xr2:uid="{E4507F59-408D-4FB0-8A67-644CB3019B49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" activeTab="2" xr2:uid="{E4507F59-408D-4FB0-8A67-644CB3019B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hématologie" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="220">
   <si>
     <t>Examens</t>
   </si>
@@ -148,15 +148,9 @@
     <t>Fibrinogène</t>
   </si>
   <si>
-    <t>GS/RH</t>
-  </si>
-  <si>
     <t>Libre</t>
   </si>
   <si>
-    <t>T. Compatibilité</t>
-  </si>
-  <si>
     <t>T. Coombs direct</t>
   </si>
   <si>
@@ -535,9 +529,6 @@
     <t>PAC</t>
   </si>
   <si>
-    <t>Electrophorèse d'HB</t>
-  </si>
-  <si>
     <t>LCR Aspect</t>
   </si>
   <si>
@@ -649,12 +640,6 @@
     <t>Syphilis</t>
   </si>
   <si>
-    <t>Blood</t>
-  </si>
-  <si>
-    <t>Puncture Fluid</t>
-  </si>
-  <si>
     <t>Sperm</t>
   </si>
   <si>
@@ -701,6 +686,9 @@
   </si>
   <si>
     <t>Numeric Range</t>
+  </si>
+  <si>
+    <t>Liquide de Ponction</t>
   </si>
 </sst>
 </file>
@@ -1060,11 +1048,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1540243A-9CAA-4A08-A50C-1E94B4501B7C}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30:E35"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1084,16 +1072,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1108,7 +1096,7 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1116,10 +1104,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>7</v>
@@ -1136,10 +1124,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1156,10 +1144,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>10</v>
@@ -1176,10 +1164,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>12</v>
@@ -1193,25 +1181,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1219,10 +1204,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
@@ -1231,90 +1216,93 @@
         <v>0</v>
       </c>
       <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>20</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K8" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="1">
-        <v>80</v>
-      </c>
-      <c r="J8" s="1">
-        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="I9" s="1">
+        <v>80</v>
+      </c>
+      <c r="J9" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I11" s="1">
         <v>32</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J11" s="1">
         <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1322,10 +1310,10 @@
         <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>12</v>
@@ -1342,10 +1330,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>12</v>
@@ -1362,10 +1350,10 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>12</v>
@@ -1382,10 +1370,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>12</v>
@@ -1402,10 +1390,10 @@
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>12</v>
@@ -1422,10 +1410,10 @@
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>7</v>
@@ -1442,10 +1430,10 @@
         <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
@@ -1462,10 +1450,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -1482,10 +1470,10 @@
         <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1493,10 +1481,10 @@
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1504,24 +1492,24 @@
         <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G23" t="s">
         <v>39</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G23" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1529,13 +1517,13 @@
         <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1543,13 +1531,13 @@
         <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1557,13 +1545,13 @@
         <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1571,13 +1559,10 @@
         <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G27" t="s">
-        <v>40</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1585,144 +1570,141 @@
         <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G28" t="s">
-        <v>40</v>
+        <v>218</v>
+      </c>
+      <c r="H28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>212</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>215</v>
+      <c r="I29" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>216</v>
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>212</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I30" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J30" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I31" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="J31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J32" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I33" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J33" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H34" t="s">
-        <v>48</v>
-      </c>
-      <c r="I34" t="s">
-        <v>61</v>
-      </c>
-      <c r="J34" t="s">
-        <v>62</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="H35" t="s">
-        <v>48</v>
-      </c>
-      <c r="I35" t="s">
-        <v>64</v>
-      </c>
-      <c r="J35" t="s">
-        <v>65</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1730,43 +1712,21 @@
         <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" t="s">
-        <v>217</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" t="s">
-        <v>217</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -1784,9 +1744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378085E8-49BE-44FC-85B7-BE860EEC5B32}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E30"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1808,16 +1768,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1832,18 +1792,18 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -1852,21 +1812,21 @@
         <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1877,39 +1837,39 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" t="s">
         <v>73</v>
-      </c>
-      <c r="J4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I5">
         <v>1.5</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K5" t="s">
         <v>15</v>
@@ -1917,22 +1877,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" t="s">
         <v>77</v>
       </c>
-      <c r="I6" t="s">
-        <v>79</v>
-      </c>
       <c r="J6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K6" t="s">
         <v>16</v>
@@ -1940,22 +1900,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K7" t="s">
         <v>16</v>
@@ -1963,22 +1923,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K8" t="s">
         <v>16</v>
@@ -1986,19 +1946,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J9">
         <v>130</v>
@@ -2009,22 +1969,22 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" t="s">
         <v>86</v>
-      </c>
-      <c r="B10" t="s">
-        <v>217</v>
-      </c>
-      <c r="E10" t="s">
-        <v>223</v>
-      </c>
-      <c r="H10" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J10" t="s">
-        <v>88</v>
       </c>
       <c r="K10" t="s">
         <v>15</v>
@@ -2032,22 +1992,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K11" t="s">
         <v>16</v>
@@ -2055,22 +2015,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E12" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K12" t="s">
         <v>16</v>
@@ -2078,19 +2038,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J13">
         <v>11</v>
@@ -2101,22 +2061,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E14" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K14" t="s">
         <v>16</v>
@@ -2124,22 +2084,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" t="s">
+        <v>218</v>
+      </c>
+      <c r="H15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I15" t="s">
         <v>95</v>
       </c>
-      <c r="B15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" t="s">
-        <v>223</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>96</v>
-      </c>
-      <c r="I15" t="s">
-        <v>97</v>
-      </c>
-      <c r="J15" t="s">
-        <v>98</v>
       </c>
       <c r="K15" t="s">
         <v>15</v>
@@ -2147,22 +2107,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E16" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K16" t="s">
         <v>16</v>
@@ -2170,16 +2130,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E17" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2190,30 +2150,30 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E18" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" t="s">
         <v>102</v>
-      </c>
-      <c r="J18" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
@@ -2221,36 +2181,36 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+      <c r="E20" t="s">
+        <v>218</v>
+      </c>
+      <c r="H20" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" t="s">
         <v>106</v>
       </c>
-      <c r="B20" t="s">
-        <v>217</v>
-      </c>
-      <c r="E20" t="s">
-        <v>223</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>107</v>
-      </c>
-      <c r="I20" t="s">
-        <v>108</v>
-      </c>
-      <c r="J20" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E21" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I21">
         <v>66</v>
@@ -2261,70 +2221,70 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+      <c r="E22" t="s">
+        <v>218</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" t="s">
         <v>111</v>
-      </c>
-      <c r="B22" t="s">
-        <v>217</v>
-      </c>
-      <c r="E22" t="s">
-        <v>223</v>
-      </c>
-      <c r="H22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I22" t="s">
-        <v>112</v>
-      </c>
-      <c r="J22" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E23" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" t="s">
+        <v>218</v>
+      </c>
+      <c r="H24" t="s">
+        <v>100</v>
+      </c>
+      <c r="I24" t="s">
         <v>114</v>
-      </c>
-      <c r="B24" t="s">
-        <v>217</v>
-      </c>
-      <c r="E24" t="s">
-        <v>223</v>
-      </c>
-      <c r="H24" t="s">
-        <v>102</v>
-      </c>
-      <c r="I24" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E25" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2335,16 +2295,16 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B26" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E26" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2355,16 +2315,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E27" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2375,47 +2335,47 @@
     </row>
     <row r="28" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E28" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E29" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E30" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2433,12 +2393,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22ADCC3-18B4-430C-9ED3-8A2AA72287E2}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B20" sqref="B20"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33:E35"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2457,16 +2417,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -2481,21 +2441,21 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I2">
         <v>70</v>
@@ -2506,16 +2466,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I3">
         <v>70</v>
@@ -2526,16 +2486,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -2546,16 +2506,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
@@ -2566,19 +2526,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J6">
         <v>7</v>
@@ -2586,64 +2546,64 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I10">
         <v>40</v>
@@ -2654,16 +2614,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I11">
         <v>500</v>
@@ -2674,39 +2634,39 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E12" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E13" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2714,36 +2674,36 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E14" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E15" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I15">
         <v>135</v>
@@ -2754,36 +2714,36 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E16" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" t="s">
         <v>53</v>
-      </c>
-      <c r="J16" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B17" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E17" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I17">
         <v>97</v>
@@ -2794,146 +2754,146 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" t="s">
+        <v>213</v>
+      </c>
+      <c r="E18" t="s">
+        <v>218</v>
+      </c>
+      <c r="H18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I18" t="s">
+        <v>146</v>
+      </c>
+      <c r="J18" t="s">
         <v>147</v>
-      </c>
-      <c r="B18" t="s">
-        <v>218</v>
-      </c>
-      <c r="E18" t="s">
-        <v>223</v>
-      </c>
-      <c r="H18" t="s">
-        <v>144</v>
-      </c>
-      <c r="I18" t="s">
-        <v>148</v>
-      </c>
-      <c r="J18" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" t="s">
+        <v>218</v>
+      </c>
+      <c r="H20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I20" t="s">
+        <v>150</v>
+      </c>
+      <c r="J20" t="s">
         <v>151</v>
-      </c>
-      <c r="B20" t="s">
-        <v>218</v>
-      </c>
-      <c r="E20" t="s">
-        <v>223</v>
-      </c>
-      <c r="H20" t="s">
-        <v>144</v>
-      </c>
-      <c r="I20" t="s">
-        <v>152</v>
-      </c>
-      <c r="J20" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E21" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22" t="s">
+        <v>212</v>
+      </c>
+      <c r="E22" t="s">
+        <v>218</v>
+      </c>
+      <c r="H22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J22" t="s">
         <v>156</v>
-      </c>
-      <c r="B22" t="s">
-        <v>217</v>
-      </c>
-      <c r="E22" t="s">
-        <v>223</v>
-      </c>
-      <c r="H22" t="s">
-        <v>157</v>
-      </c>
-      <c r="J22" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E23" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E24" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E25" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E26" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I26">
         <v>38</v>
@@ -2944,16 +2904,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E27" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I27">
         <v>60</v>
@@ -2964,69 +2924,75 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B28" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E28" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B29" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E29" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B30" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E30" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E31" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" t="s">
+        <v>219</v>
+      </c>
+      <c r="E32" t="s">
+        <v>218</v>
+      </c>
+      <c r="H32" t="s">
+        <v>168</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
         <v>169</v>
-      </c>
-      <c r="B32" t="s">
-        <v>207</v>
-      </c>
-      <c r="E32" t="s">
-        <v>215</v>
-      </c>
-      <c r="G32" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3034,109 +3000,89 @@
         <v>170</v>
       </c>
       <c r="B33" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E33" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H33" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
-      <c r="J33" t="s">
-        <v>172</v>
+      <c r="J33">
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B34" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E34" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H34" t="s">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B35" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E35" t="s">
-        <v>223</v>
-      </c>
-      <c r="H35" t="s">
-        <v>48</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>40</v>
+        <v>210</v>
+      </c>
+      <c r="G35" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E36" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E37" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>177</v>
-      </c>
-      <c r="B38" t="s">
-        <v>207</v>
-      </c>
-      <c r="E38" t="s">
-        <v>215</v>
-      </c>
-      <c r="G38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E24:E25 E31:E32 E36:E1048576" xr:uid="{1AABA173-1840-4CD3-B40C-7980058AC08A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E24:E25 E35:E1048576 E31" xr:uid="{1AABA173-1840-4CD3-B40C-7980058AC08A}">
       <formula1>"Auto Complete, Free Text, Numeric, Alpha Numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23 E26:E30 E33:E35" xr:uid="{A95DF725-4190-4227-82FE-7A3DF9F148E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23 E26:E30 E32:E34" xr:uid="{A95DF725-4190-4227-82FE-7A3DF9F148E8}">
       <formula1>"Auto Complete, Free Text, Numeric Range, Alpha Numeric"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3149,7 +3095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5883E73-6570-469C-B00B-2AE9C0B4CDEF}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9:E15"/>
     </sheetView>
   </sheetViews>
@@ -3170,16 +3116,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -3194,156 +3140,156 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E10" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E11" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I11">
         <v>2001</v>
@@ -3354,19 +3300,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E12" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I12">
         <v>4001</v>
@@ -3377,50 +3323,50 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" t="s">
+        <v>210</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" t="s">
+        <v>186</v>
+      </c>
+      <c r="J13" t="s">
         <v>188</v>
-      </c>
-      <c r="B13" t="s">
-        <v>216</v>
-      </c>
-      <c r="E13" t="s">
-        <v>215</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" t="s">
-        <v>189</v>
-      </c>
-      <c r="J13" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E14" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E15" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3437,8 +3383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058C4361-8A64-4A1B-8C01-6330C5F7CB23}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3457,16 +3403,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -3481,41 +3427,41 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J2" t="s">
         <v>217</v>
-      </c>
-      <c r="E2" t="s">
-        <v>223</v>
-      </c>
-      <c r="I2" t="s">
-        <v>221</v>
-      </c>
-      <c r="J2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J3">
         <v>5</v>
@@ -3523,36 +3469,36 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -3563,16 +3509,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -3583,58 +3529,58 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B10" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test update script
</commit_message>
<xml_diff>
--- a/storage/EXAMENS.xlsx
+++ b/storage/EXAMENS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\var\www\nlims_controller_global\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC4318C-B944-4B13-948A-2362675314EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D612B65E-4B29-4B84-ACE5-C35135C2EBD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" activeTab="2" xr2:uid="{E4507F59-408D-4FB0-8A67-644CB3019B49}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="221">
   <si>
     <t>Examens</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Fibrinogène</t>
+  </si>
+  <si>
+    <t>GS/RH</t>
   </si>
   <si>
     <t>Libre</t>
@@ -1048,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1540243A-9CAA-4A08-A50C-1E94B4501B7C}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
@@ -1072,16 +1075,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1096,7 +1099,7 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1104,10 +1107,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>7</v>
@@ -1124,10 +1127,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
@@ -1144,10 +1147,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>10</v>
@@ -1164,10 +1167,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>12</v>
@@ -1184,10 +1187,10 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -1204,10 +1207,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
@@ -1227,10 +1230,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
@@ -1250,10 +1253,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>18</v>
@@ -1270,10 +1273,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>20</v>
@@ -1290,10 +1293,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>10</v>
@@ -1310,10 +1313,10 @@
         <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>12</v>
@@ -1330,10 +1333,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>12</v>
@@ -1350,10 +1353,10 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>12</v>
@@ -1370,10 +1373,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>12</v>
@@ -1390,10 +1393,10 @@
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>12</v>
@@ -1410,10 +1413,10 @@
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>7</v>
@@ -1430,10 +1433,10 @@
         <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
@@ -1450,10 +1453,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
@@ -1470,10 +1473,10 @@
         <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1481,10 +1484,10 @@
         <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1492,24 +1495,24 @@
         <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G23" t="s">
         <v>40</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G23" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1517,13 +1520,13 @@
         <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="G24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1531,13 +1534,13 @@
         <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1545,13 +1548,13 @@
         <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1559,10 +1562,13 @@
         <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>210</v>
+      <c r="G27" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1570,130 +1576,130 @@
         <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H28" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" t="s">
-        <v>47</v>
-      </c>
-      <c r="J28" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I29" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" t="s">
         <v>49</v>
-      </c>
-      <c r="B29" t="s">
-        <v>212</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H29" t="s">
-        <v>46</v>
-      </c>
-      <c r="I29" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>213</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H30" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" t="s">
         <v>52</v>
-      </c>
-      <c r="B30" t="s">
-        <v>212</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H30" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" t="s">
-        <v>53</v>
-      </c>
-      <c r="J30" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
+        <v>213</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H31" t="s">
+        <v>47</v>
+      </c>
+      <c r="I31" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31" t="s">
         <v>55</v>
-      </c>
-      <c r="B31" t="s">
-        <v>212</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H32" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32" t="s">
+        <v>57</v>
+      </c>
+      <c r="J32" t="s">
         <v>58</v>
-      </c>
-      <c r="B32" t="s">
-        <v>212</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H32" t="s">
-        <v>46</v>
-      </c>
-      <c r="I32" t="s">
-        <v>59</v>
-      </c>
-      <c r="J32" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>213</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H33" t="s">
+        <v>47</v>
+      </c>
+      <c r="I33" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" t="s">
         <v>61</v>
-      </c>
-      <c r="B33" t="s">
-        <v>212</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H33" t="s">
-        <v>46</v>
-      </c>
-      <c r="I33" t="s">
-        <v>62</v>
-      </c>
-      <c r="J33" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>213</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H34" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" t="s">
         <v>64</v>
-      </c>
-      <c r="B34" t="s">
-        <v>212</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1701,10 +1707,10 @@
         <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1712,21 +1718,32 @@
         <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
         <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
+        <v>213</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1745,8 +1762,8 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1768,16 +1785,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -1792,18 +1809,18 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -1812,21 +1829,21 @@
         <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1837,39 +1854,39 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" t="s">
+        <v>219</v>
+      </c>
+      <c r="H4" t="s">
         <v>72</v>
       </c>
-      <c r="B4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H4" t="s">
-        <v>71</v>
-      </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I5">
         <v>1.5</v>
       </c>
       <c r="J5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s">
         <v>15</v>
@@ -1877,22 +1894,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K6" t="s">
         <v>16</v>
@@ -1900,22 +1917,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K7" t="s">
         <v>16</v>
@@ -1923,22 +1940,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K8" t="s">
         <v>16</v>
@@ -1946,19 +1963,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J9">
         <v>130</v>
@@ -1969,22 +1986,22 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K10" t="s">
         <v>15</v>
@@ -1992,22 +2009,22 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K11" t="s">
         <v>16</v>
@@ -2015,22 +2032,22 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K12" t="s">
         <v>16</v>
@@ -2038,19 +2055,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J13">
         <v>11</v>
@@ -2061,22 +2078,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K14" t="s">
         <v>16</v>
@@ -2084,22 +2101,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E15" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K15" t="s">
         <v>15</v>
@@ -2107,22 +2124,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K16" t="s">
         <v>16</v>
@@ -2130,16 +2147,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2150,30 +2167,30 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" t="s">
+        <v>213</v>
+      </c>
+      <c r="E18" t="s">
+        <v>219</v>
+      </c>
+      <c r="H18" t="s">
         <v>101</v>
       </c>
-      <c r="B18" t="s">
-        <v>212</v>
-      </c>
-      <c r="E18" t="s">
-        <v>218</v>
-      </c>
-      <c r="H18" t="s">
-        <v>100</v>
-      </c>
       <c r="J18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
@@ -2181,36 +2198,36 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B20" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H21" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I21">
         <v>66</v>
@@ -2221,70 +2238,70 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E22" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E23" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E24" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E25" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2295,16 +2312,16 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E26" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2315,16 +2332,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2335,47 +2352,47 @@
     </row>
     <row r="28" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E29" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B30" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2398,7 +2415,7 @@
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B20" sqref="B20"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2417,16 +2434,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -2441,21 +2458,21 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I2">
         <v>70</v>
@@ -2466,16 +2483,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H3" t="s">
         <v>124</v>
-      </c>
-      <c r="B3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="H3" t="s">
-        <v>123</v>
       </c>
       <c r="I3">
         <v>70</v>
@@ -2486,16 +2503,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I4">
         <v>15</v>
@@ -2506,16 +2523,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
@@ -2526,19 +2543,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J6">
         <v>7</v>
@@ -2546,64 +2563,64 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I10">
         <v>40</v>
@@ -2614,16 +2631,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I11">
         <v>500</v>
@@ -2634,39 +2651,39 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" t="s">
+        <v>219</v>
+      </c>
+      <c r="H13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" t="s">
         <v>138</v>
-      </c>
-      <c r="B13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E13" t="s">
-        <v>218</v>
-      </c>
-      <c r="H13" t="s">
-        <v>123</v>
-      </c>
-      <c r="I13" t="s">
-        <v>137</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2674,36 +2691,36 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E15" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H15" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I15">
         <v>135</v>
@@ -2714,36 +2731,36 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" t="s">
+        <v>219</v>
+      </c>
+      <c r="H16" t="s">
         <v>143</v>
       </c>
-      <c r="B16" t="s">
-        <v>213</v>
-      </c>
-      <c r="E16" t="s">
-        <v>218</v>
-      </c>
-      <c r="H16" t="s">
-        <v>142</v>
-      </c>
       <c r="I16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H17" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I17">
         <v>97</v>
@@ -2754,146 +2771,146 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E18" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B20" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E20" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J20" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H21" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E22" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E23" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E25" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E26" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I26">
         <v>38</v>
@@ -2904,16 +2921,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B27" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E27" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I27">
         <v>60</v>
@@ -2924,89 +2941,89 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E29" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H29" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" t="s">
+        <v>213</v>
+      </c>
+      <c r="E30" t="s">
+        <v>219</v>
+      </c>
+      <c r="H30" t="s">
         <v>165</v>
-      </c>
-      <c r="B30" t="s">
-        <v>212</v>
-      </c>
-      <c r="E30" t="s">
-        <v>218</v>
-      </c>
-      <c r="H30" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B31" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E31" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E32" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I32">
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B33" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E33" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H33" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -3017,16 +3034,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B34" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E34" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -3037,44 +3054,44 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B35" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E35" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B36" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E36" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B37" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E37" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3116,16 +3133,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -3140,156 +3157,156 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" t="s">
         <v>211</v>
       </c>
-      <c r="E9" t="s">
-        <v>210</v>
-      </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" t="s">
         <v>211</v>
       </c>
-      <c r="E10" t="s">
-        <v>210</v>
-      </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" t="s">
         <v>211</v>
       </c>
-      <c r="E11" t="s">
-        <v>210</v>
-      </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I11">
         <v>2001</v>
@@ -3300,19 +3317,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
+        <v>212</v>
+      </c>
+      <c r="E12" t="s">
         <v>211</v>
       </c>
-      <c r="E12" t="s">
-        <v>210</v>
-      </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I12">
         <v>4001</v>
@@ -3323,50 +3340,50 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B13" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" t="s">
         <v>211</v>
       </c>
-      <c r="E13" t="s">
-        <v>210</v>
-      </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J13" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E15" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3383,9 +3400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058C4361-8A64-4A1B-8C01-6330C5F7CB23}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -3403,16 +3418,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -3427,41 +3442,41 @@
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I2" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" t="s">
         <v>218</v>
-      </c>
-      <c r="I2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J3">
         <v>5</v>
@@ -3469,36 +3484,36 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -3509,16 +3524,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="H6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -3529,58 +3544,58 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E10" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3593,5 +3608,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated tests with VL
</commit_message>
<xml_diff>
--- a/storage/EXAMENS.xlsx
+++ b/storage/EXAMENS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\var\www\nlims_controller_global\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-18.04\var\www\nlims_controller_global\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D612B65E-4B29-4B84-ACE5-C35135C2EBD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD240A2-D671-4FBC-9F6A-61FFBACD9A00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10296" activeTab="2" xr2:uid="{E4507F59-408D-4FB0-8A67-644CB3019B49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="6828" activeTab="4" xr2:uid="{E4507F59-408D-4FB0-8A67-644CB3019B49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hématologie" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="223">
   <si>
     <t>Examens</t>
   </si>
@@ -692,6 +692,12 @@
   </si>
   <si>
     <t>Liquide de Ponction</t>
+  </si>
+  <si>
+    <t>Charge Virale(CV)</t>
+  </si>
+  <si>
+    <t>copies/ml</t>
   </si>
 </sst>
 </file>
@@ -2412,7 +2418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22ADCC3-18B4-430C-9ED3-8A2AA72287E2}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B20" sqref="B20"/>
       <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
@@ -3398,9 +3404,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058C4361-8A64-4A1B-8C01-6330C5F7CB23}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -3598,12 +3606,26 @@
         <v>40</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11" t="s">
+        <v>219</v>
+      </c>
+      <c r="H11" t="s">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E7:E1048576" xr:uid="{4135F017-CEC7-4C3E-806D-4174A0F0139B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E7:E10 E12:E1048576" xr:uid="{4135F017-CEC7-4C3E-806D-4174A0F0139B}">
       <formula1>"Auto Complete, Free Text, Numeric, Alpha Numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{B7C0CFF6-5AAA-4090-8A80-5FED46016112}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6 E11" xr:uid="{B7C0CFF6-5AAA-4090-8A80-5FED46016112}">
       <formula1>"Auto Complete, Free Text, Numeric Range, Alpha Numeric"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>